<commit_message>
Added MSI and busy curser feature
</commit_message>
<xml_diff>
--- a/US_Industry.xlsx
+++ b/US_Industry.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mrinal Bera\PycharmProjects\ChemMat_User_Stats\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="18" windowWidth="16098" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -250,11 +255,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +323,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -364,7 +377,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -396,9 +409,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -430,6 +444,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -605,14 +620,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="14.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.15625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.9453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5234375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.3671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.62890625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.05078125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="38.47265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,7 +695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>237982</v>
       </c>
@@ -712,7 +742,7 @@
         <v>80603</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>244570</v>
       </c>
@@ -732,7 +762,7 @@
         <v>49</v>
       </c>
       <c r="G3" s="2">
-        <v>42239.69038194444</v>
+        <v>42239.690381944441</v>
       </c>
       <c r="H3" t="s">
         <v>51</v>
@@ -759,7 +789,7 @@
         <v>95540</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>279756</v>
       </c>
@@ -806,7 +836,7 @@
         <v>106900</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>290344</v>
       </c>
@@ -853,7 +883,7 @@
         <v>121777</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>292449</v>
       </c>
@@ -900,7 +930,7 @@
         <v>121777</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>296828</v>
       </c>
@@ -947,7 +977,7 @@
         <v>132822</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>40625</v>
       </c>
@@ -994,7 +1024,7 @@
         <v>121777</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>67422</v>
       </c>
@@ -1014,7 +1044,7 @@
         <v>49</v>
       </c>
       <c r="G9" s="2">
-        <v>41686.66666666666</v>
+        <v>41686.666666666657</v>
       </c>
       <c r="H9" t="s">
         <v>51</v>
@@ -1041,7 +1071,7 @@
         <v>79672</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>82549</v>
       </c>
@@ -1061,7 +1091,7 @@
         <v>49</v>
       </c>
       <c r="G10" s="2">
-        <v>41812.35416666666</v>
+        <v>41812.354166666657</v>
       </c>
       <c r="H10" t="s">
         <v>51</v>
@@ -1088,7 +1118,7 @@
         <v>82805</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>83177</v>
       </c>
@@ -1108,7 +1138,7 @@
         <v>50</v>
       </c>
       <c r="G11" s="2">
-        <v>42121.36287037037</v>
+        <v>42121.362870370373</v>
       </c>
       <c r="H11" t="s">
         <v>51</v>
@@ -1135,7 +1165,7 @@
         <v>91914</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>88283</v>
       </c>
@@ -1155,7 +1185,7 @@
         <v>49</v>
       </c>
       <c r="G12" s="2">
-        <v>41978.60416666666</v>
+        <v>41978.604166666657</v>
       </c>
       <c r="H12" t="s">
         <v>51</v>

</xml_diff>